<commit_message>
Excel file converted to CSV from gaze_tracking.py, data appending
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,22 +420,22 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>668</v>
+        <v>726</v>
       </c>
       <c r="C2">
-        <v>379</v>
+        <v>446</v>
       </c>
       <c r="D2">
-        <v>776</v>
+        <v>828</v>
       </c>
       <c r="E2">
-        <v>379</v>
+        <v>442</v>
       </c>
       <c r="F2">
-        <v>523.5</v>
+        <v>586</v>
       </c>
       <c r="G2">
-        <v>577.5</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,22 +443,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>665</v>
+        <v>721</v>
       </c>
       <c r="C3">
-        <v>376</v>
+        <v>446</v>
       </c>
       <c r="D3">
-        <v>775</v>
+        <v>822</v>
       </c>
       <c r="E3">
-        <v>377</v>
+        <v>440</v>
       </c>
       <c r="F3">
-        <v>520.5</v>
+        <v>583.5</v>
       </c>
       <c r="G3">
-        <v>576</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,22 +466,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>668</v>
+        <v>722</v>
       </c>
       <c r="C4">
-        <v>374</v>
+        <v>446</v>
       </c>
       <c r="D4">
-        <v>780</v>
+        <v>824</v>
       </c>
       <c r="E4">
-        <v>375</v>
+        <v>441</v>
       </c>
       <c r="F4">
-        <v>521</v>
+        <v>584</v>
       </c>
       <c r="G4">
-        <v>577.5</v>
+        <v>632.5</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,22 +489,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>670</v>
+        <v>721</v>
       </c>
       <c r="C5">
-        <v>375</v>
+        <v>445</v>
       </c>
       <c r="D5">
-        <v>781</v>
+        <v>822</v>
       </c>
       <c r="E5">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="F5">
-        <v>522.5</v>
+        <v>583</v>
       </c>
       <c r="G5">
-        <v>578.5</v>
+        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,22 +512,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>671</v>
+        <v>720</v>
       </c>
       <c r="C6">
-        <v>373</v>
+        <v>445</v>
       </c>
       <c r="D6">
-        <v>782</v>
+        <v>823</v>
       </c>
       <c r="E6">
-        <v>374</v>
+        <v>442</v>
       </c>
       <c r="F6">
-        <v>522</v>
+        <v>582.5</v>
       </c>
       <c r="G6">
-        <v>578</v>
+        <v>632.5</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -535,22 +535,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>673</v>
+        <v>725</v>
       </c>
       <c r="C7">
-        <v>375</v>
+        <v>442</v>
       </c>
       <c r="D7">
-        <v>784</v>
+        <v>829</v>
       </c>
       <c r="E7">
-        <v>377</v>
+        <v>438</v>
       </c>
       <c r="F7">
-        <v>524</v>
+        <v>583.5</v>
       </c>
       <c r="G7">
-        <v>580.5</v>
+        <v>633.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,22 +558,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>674</v>
+        <v>726</v>
       </c>
       <c r="C8">
-        <v>374</v>
+        <v>442</v>
       </c>
       <c r="D8">
-        <v>785</v>
+        <v>831</v>
       </c>
       <c r="E8">
-        <v>375</v>
+        <v>437</v>
       </c>
       <c r="F8">
-        <v>524</v>
+        <v>584</v>
       </c>
       <c r="G8">
-        <v>580</v>
+        <v>634</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -581,22 +581,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>675</v>
+        <v>724</v>
       </c>
       <c r="C9">
-        <v>374</v>
+        <v>444</v>
       </c>
       <c r="D9">
-        <v>786</v>
+        <v>829</v>
       </c>
       <c r="E9">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="F9">
-        <v>524.5</v>
+        <v>584</v>
       </c>
       <c r="G9">
-        <v>581</v>
+        <v>634.5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -604,22 +604,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>677</v>
+        <v>725</v>
       </c>
       <c r="C10">
-        <v>372</v>
+        <v>442</v>
       </c>
       <c r="D10">
-        <v>789</v>
+        <v>830</v>
       </c>
       <c r="E10">
-        <v>375</v>
+        <v>438</v>
       </c>
       <c r="F10">
-        <v>524.5</v>
+        <v>583.5</v>
       </c>
       <c r="G10">
-        <v>582</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -627,22 +627,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>681</v>
+        <v>725</v>
       </c>
       <c r="C11">
-        <v>374</v>
+        <v>443</v>
       </c>
       <c r="D11">
-        <v>793</v>
+        <v>829</v>
       </c>
       <c r="E11">
-        <v>376</v>
+        <v>438</v>
       </c>
       <c r="F11">
-        <v>527.5</v>
+        <v>584</v>
       </c>
       <c r="G11">
-        <v>584.5</v>
+        <v>633.5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -650,22 +650,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>681</v>
+        <v>740</v>
       </c>
       <c r="C12">
-        <v>375</v>
+        <v>443</v>
       </c>
       <c r="D12">
-        <v>792</v>
+        <v>841</v>
       </c>
       <c r="E12">
-        <v>378</v>
+        <v>440</v>
       </c>
       <c r="F12">
-        <v>528</v>
+        <v>591.5</v>
       </c>
       <c r="G12">
-        <v>585</v>
+        <v>640.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -673,22 +673,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>685</v>
+        <v>742</v>
       </c>
       <c r="C13">
-        <v>377</v>
+        <v>440</v>
       </c>
       <c r="D13">
-        <v>797</v>
+        <v>844</v>
       </c>
       <c r="E13">
-        <v>380</v>
+        <v>438</v>
       </c>
       <c r="F13">
-        <v>531</v>
+        <v>591</v>
       </c>
       <c r="G13">
-        <v>588.5</v>
+        <v>641</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -696,344 +696,22 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>681</v>
+        <v>729</v>
       </c>
       <c r="C14">
-        <v>376</v>
+        <v>443</v>
       </c>
       <c r="D14">
-        <v>793</v>
+        <v>831</v>
       </c>
       <c r="E14">
-        <v>378</v>
+        <v>438</v>
       </c>
       <c r="F14">
-        <v>528.5</v>
+        <v>586</v>
       </c>
       <c r="G14">
-        <v>585.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>678</v>
-      </c>
-      <c r="C15">
-        <v>377</v>
-      </c>
-      <c r="D15">
-        <v>789</v>
-      </c>
-      <c r="E15">
-        <v>379</v>
-      </c>
-      <c r="F15">
-        <v>527.5</v>
-      </c>
-      <c r="G15">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>677</v>
-      </c>
-      <c r="C16">
-        <v>375</v>
-      </c>
-      <c r="D16">
-        <v>789</v>
-      </c>
-      <c r="E16">
-        <v>377</v>
-      </c>
-      <c r="F16">
-        <v>526</v>
-      </c>
-      <c r="G16">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>679</v>
-      </c>
-      <c r="C17">
-        <v>375</v>
-      </c>
-      <c r="D17">
-        <v>791</v>
-      </c>
-      <c r="E17">
-        <v>377</v>
-      </c>
-      <c r="F17">
-        <v>527</v>
-      </c>
-      <c r="G17">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>674</v>
-      </c>
-      <c r="C18">
-        <v>382</v>
-      </c>
-      <c r="D18">
-        <v>784</v>
-      </c>
-      <c r="E18">
-        <v>384</v>
-      </c>
-      <c r="F18">
-        <v>528</v>
-      </c>
-      <c r="G18">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>678</v>
-      </c>
-      <c r="C19">
-        <v>374</v>
-      </c>
-      <c r="D19">
-        <v>788</v>
-      </c>
-      <c r="E19">
-        <v>376</v>
-      </c>
-      <c r="F19">
-        <v>526</v>
-      </c>
-      <c r="G19">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>677</v>
-      </c>
-      <c r="C20">
-        <v>372</v>
-      </c>
-      <c r="D20">
-        <v>787</v>
-      </c>
-      <c r="E20">
-        <v>375</v>
-      </c>
-      <c r="F20">
-        <v>524.5</v>
-      </c>
-      <c r="G20">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>676</v>
-      </c>
-      <c r="C21">
-        <v>372</v>
-      </c>
-      <c r="D21">
-        <v>787</v>
-      </c>
-      <c r="E21">
-        <v>376</v>
-      </c>
-      <c r="F21">
-        <v>524</v>
-      </c>
-      <c r="G21">
-        <v>581.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>668</v>
-      </c>
-      <c r="C22">
-        <v>371</v>
-      </c>
-      <c r="D22">
-        <v>780</v>
-      </c>
-      <c r="E22">
-        <v>374</v>
-      </c>
-      <c r="F22">
-        <v>519.5</v>
-      </c>
-      <c r="G22">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>667</v>
-      </c>
-      <c r="C23">
-        <v>372</v>
-      </c>
-      <c r="D23">
-        <v>779</v>
-      </c>
-      <c r="E23">
-        <v>374</v>
-      </c>
-      <c r="F23">
-        <v>519.5</v>
-      </c>
-      <c r="G23">
-        <v>576.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>665</v>
-      </c>
-      <c r="C24">
-        <v>372</v>
-      </c>
-      <c r="D24">
-        <v>777</v>
-      </c>
-      <c r="E24">
-        <v>375</v>
-      </c>
-      <c r="F24">
-        <v>518.5</v>
-      </c>
-      <c r="G24">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>666</v>
-      </c>
-      <c r="C25">
-        <v>372</v>
-      </c>
-      <c r="D25">
-        <v>777</v>
-      </c>
-      <c r="E25">
-        <v>374</v>
-      </c>
-      <c r="F25">
-        <v>519</v>
-      </c>
-      <c r="G25">
-        <v>575.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>667</v>
-      </c>
-      <c r="C26">
-        <v>371</v>
-      </c>
-      <c r="D26">
-        <v>777</v>
-      </c>
-      <c r="E26">
-        <v>374</v>
-      </c>
-      <c r="F26">
-        <v>519</v>
-      </c>
-      <c r="G26">
-        <v>575.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>668</v>
-      </c>
-      <c r="C27">
-        <v>370</v>
-      </c>
-      <c r="D27">
-        <v>781</v>
-      </c>
-      <c r="E27">
-        <v>373</v>
-      </c>
-      <c r="F27">
-        <v>519</v>
-      </c>
-      <c r="G27">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>666</v>
-      </c>
-      <c r="C28">
-        <v>371</v>
-      </c>
-      <c r="D28">
-        <v>777</v>
-      </c>
-      <c r="E28">
-        <v>373</v>
-      </c>
-      <c r="F28">
-        <v>518.5</v>
-      </c>
-      <c r="G28">
-        <v>575</v>
+        <v>634.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>